<commit_message>
HF changes with diffrent workflow
</commit_message>
<xml_diff>
--- a/Data/Reportfor_PreQc_status.xlsx
+++ b/Data/Reportfor_PreQc_status.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
   <x:si>
     <x:t>Module</x:t>
   </x:si>
@@ -143,6 +143,156 @@
   </x:si>
   <x:si>
     <x:t>19-01-2021 06:37:51 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21-01-2021 05:11:30 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21-01-2021 05:11:56 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21-01-2021 05:12:11 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21-01-2021 05:12:23 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>House format (HF) medialevel</x:t>
+  </x:si>
+  <x:si>
+    <x:t>House format (HF) medialevel is completed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21-01-2021 05:12:38 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21-01-2021 05:16:11 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21-01-2021 05:16:40 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21-01-2021 05:16:54 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21-01-2021 05:17:07 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21-01-2021 05:17:21 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21-01-2021 05:18:15 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21-01-2021 05:18:43 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21-01-2021 05:18:58 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21-01-2021 05:19:10 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21-01-2021 05:19:25 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21-01-2021 05:19:40 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21-01-2021 05:19:45 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21-01-2021 05:20:16 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21-01-2021 05:28:26 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21-01-2021 05:28:54 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21-01-2021 05:29:09 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21-01-2021 05:29:21 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21-01-2021 05:29:36 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 12:39:04 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 12:39:44 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 12:39:59 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 12:40:11 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 12:59:50 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 01:00:18 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 03:55:02 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 03:55:30 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 03:55:58 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 03:56:11 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ingest status in DM level</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ingest status in DM level is completed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 03:56:25 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 03:56:40 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 03:56:45 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 04:01:25 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 04:01:53 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 04:02:07 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 04:02:20 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 04:02:34 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 04:02:49 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 04:02:54 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DateTime.Now.Date.ToString("dd-MM-yyyy")</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 04:14:54 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 04:15:24 PM</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -822,6 +972,641 @@
         <x:v>40</x:v>
       </x:c>
     </x:row>
+    <x:row r="23" spans="1:4">
+      <x:c r="A23" s="4" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B23" s="4" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C23" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D23" s="4" t="s">
+        <x:v>41</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:4">
+      <x:c r="A24" s="4" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B24" s="4" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C24" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D24" s="4" t="s">
+        <x:v>42</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:4">
+      <x:c r="A25" s="4" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B25" s="4" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C25" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D25" s="4" t="s">
+        <x:v>43</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:4">
+      <x:c r="A26" s="4" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B26" s="4" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C26" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D26" s="4" t="s">
+        <x:v>44</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:4">
+      <x:c r="A27" s="4" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="B27" s="4" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="C27" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D27" s="4" t="s">
+        <x:v>47</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:4">
+      <x:c r="A28" s="4" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B28" s="4" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C28" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D28" s="4" t="s">
+        <x:v>48</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:4">
+      <x:c r="A29" s="4" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B29" s="4" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C29" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D29" s="4" t="s">
+        <x:v>49</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:4">
+      <x:c r="A30" s="4" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B30" s="4" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C30" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D30" s="4" t="s">
+        <x:v>50</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:4">
+      <x:c r="A31" s="4" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B31" s="4" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C31" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D31" s="4" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:4">
+      <x:c r="A32" s="4" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="B32" s="4" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="C32" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D32" s="4" t="s">
+        <x:v>52</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:4">
+      <x:c r="A33" s="4" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B33" s="4" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C33" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D33" s="4" t="s">
+        <x:v>53</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:4">
+      <x:c r="A34" s="4" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B34" s="4" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C34" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D34" s="4" t="s">
+        <x:v>54</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:4">
+      <x:c r="A35" s="4" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B35" s="4" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C35" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D35" s="4" t="s">
+        <x:v>55</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:4">
+      <x:c r="A36" s="4" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B36" s="4" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C36" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D36" s="4" t="s">
+        <x:v>56</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:4">
+      <x:c r="A37" s="4" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="B37" s="4" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="C37" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D37" s="4" t="s">
+        <x:v>57</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:4">
+      <x:c r="A38" s="4" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B38" s="4" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C38" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D38" s="4" t="s">
+        <x:v>58</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:4">
+      <x:c r="A39" s="4" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B39" s="4" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C39" s="4" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="D39" s="4" t="s">
+        <x:v>59</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:4">
+      <x:c r="A40" s="4" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="B40" s="4" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="C40" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D40" s="4" t="s">
+        <x:v>60</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:4">
+      <x:c r="A41" s="4" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B41" s="4" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C41" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D41" s="4" t="s">
+        <x:v>61</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42" spans="1:4">
+      <x:c r="A42" s="4" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B42" s="4" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C42" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D42" s="4" t="s">
+        <x:v>62</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43" spans="1:4">
+      <x:c r="A43" s="4" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B43" s="4" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C43" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D43" s="4" t="s">
+        <x:v>63</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44" spans="1:4">
+      <x:c r="A44" s="4" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B44" s="4" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C44" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D44" s="4" t="s">
+        <x:v>64</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="45" spans="1:4">
+      <x:c r="A45" s="4" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="B45" s="4" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="C45" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D45" s="4" t="s">
+        <x:v>65</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="46" spans="1:4">
+      <x:c r="A46" s="4" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B46" s="4" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C46" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D46" s="4" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="47" spans="1:4">
+      <x:c r="A47" s="4" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B47" s="4" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C47" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D47" s="4" t="s">
+        <x:v>67</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="48" spans="1:4">
+      <x:c r="A48" s="4" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B48" s="4" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C48" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D48" s="4" t="s">
+        <x:v>68</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="49" spans="1:4">
+      <x:c r="A49" s="4" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B49" s="4" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C49" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D49" s="4" t="s">
+        <x:v>69</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="50" spans="1:4">
+      <x:c r="A50" s="4" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B50" s="4" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C50" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D50" s="4" t="s">
+        <x:v>70</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="51" spans="1:4">
+      <x:c r="A51" s="4" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B51" s="4" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C51" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D51" s="4" t="s">
+        <x:v>71</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="52" spans="1:4">
+      <x:c r="A52" s="4" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B52" s="4" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C52" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D52" s="4" t="s">
+        <x:v>72</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="53" spans="1:4">
+      <x:c r="A53" s="4" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B53" s="4" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C53" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D53" s="4" t="s">
+        <x:v>73</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="54" spans="1:4">
+      <x:c r="A54" s="4" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B54" s="4" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C54" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D54" s="4" t="s">
+        <x:v>74</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="55" spans="1:4">
+      <x:c r="A55" s="4" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B55" s="4" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C55" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D55" s="4" t="s">
+        <x:v>75</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="56" spans="1:4">
+      <x:c r="A56" s="4" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="B56" s="4" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="C56" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D56" s="4" t="s">
+        <x:v>78</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="57" spans="1:4">
+      <x:c r="A57" s="4" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B57" s="4" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C57" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D57" s="4" t="s">
+        <x:v>79</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="58" spans="1:4">
+      <x:c r="A58" s="4" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B58" s="4" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C58" s="4" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="D58" s="4" t="s">
+        <x:v>80</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="59" spans="1:4">
+      <x:c r="A59" s="4" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B59" s="4" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C59" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D59" s="4" t="s">
+        <x:v>81</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="60" spans="1:4">
+      <x:c r="A60" s="4" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B60" s="4" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C60" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D60" s="4" t="s">
+        <x:v>82</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="61" spans="1:4">
+      <x:c r="A61" s="4" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B61" s="4" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C61" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D61" s="4" t="s">
+        <x:v>83</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="62" spans="1:4">
+      <x:c r="A62" s="4" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B62" s="4" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C62" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D62" s="4" t="s">
+        <x:v>84</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="63" spans="1:4">
+      <x:c r="A63" s="4" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="B63" s="4" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="C63" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D63" s="4" t="s">
+        <x:v>85</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="64" spans="1:4">
+      <x:c r="A64" s="4" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B64" s="4" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C64" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D64" s="4" t="s">
+        <x:v>86</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="65" spans="1:4">
+      <x:c r="A65" s="4" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B65" s="4" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C65" s="4" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="D65" s="4" t="s">
+        <x:v>87</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="66" spans="1:4">
+      <x:c r="D66" s="4" t="s">
+        <x:v>88</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="67" spans="1:4">
+      <x:c r="A67" s="4" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B67" s="4" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C67" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D67" s="4" t="s">
+        <x:v>89</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="68" spans="1:4">
+      <x:c r="A68" s="4" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B68" s="4" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C68" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D68" s="4" t="s">
+        <x:v>90</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>